<commit_message>
tham nien, khen thuong, ky luat
</commit_message>
<xml_diff>
--- a/assets/SourceFile/chamcong_t05_2022.xlsx
+++ b/assets/SourceFile/chamcong_t05_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\BTL_PHP\hr-management\assets\SourceFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D20DA34-18E9-456E-A848-A978806EB17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A6DF9F-EA27-40C0-A357-40F356666304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="25">
   <si>
     <t>Mã NV</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>Tổng</t>
-  </si>
-  <si>
-    <t>Đào Đức Tuấn</t>
   </si>
   <si>
     <t>x</t>
@@ -155,115 +152,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0"/>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <sz val="10"/>
@@ -588,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH21"/>
+  <dimension ref="A1:AH20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AD21" sqref="AD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -709,628 +598,628 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH2" s="1">
-        <f t="shared" ref="AH2:AH21" si="0">COUNTIF(C2:AG2, "x")</f>
-        <v>26</v>
+        <f t="shared" ref="AH2:AH20" si="0">COUNTIF(C2:AG2, "x")</f>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH3" s="1">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH4" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AG5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH5" s="1">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AG6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH6" s="1">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH7" s="1">
         <f t="shared" si="0"/>
@@ -1339,313 +1228,264 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P8" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>4</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
       <c r="AH8" s="1">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH9" s="1">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH10" s="1">
         <f t="shared" si="0"/>
@@ -1654,628 +1494,628 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH11" s="1">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AE12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH12" s="1">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH13" s="1">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH14" s="1">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH15" s="1">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH16" s="1">
         <f t="shared" si="0"/>
@@ -2284,103 +2124,103 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH17" s="1">
         <f t="shared" si="0"/>
@@ -2389,103 +2229,103 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH18" s="1">
         <f t="shared" si="0"/>
@@ -2494,315 +2334,210 @@
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z19" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AA19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH19" s="1">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P20" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Z20" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AF20" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG20" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="AG20" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="AH20" s="1">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="X21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF21" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH21" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -2810,11 +2545,11 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"v"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"CN"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
-      <formula>"v"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>